<commit_message>
Update question numbers in every question as well as result section
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/modeltest_v1.xlsx
+++ b/app/src/main/res/raw/modeltest_v1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="metadata_modeltest" sheetId="3" r:id="rId1"/>
@@ -2891,7 +2891,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2933,6 +2933,11 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2948,7 +2953,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2982,11 +2987,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3016,6 +3049,12 @@
     <xf numFmtId="21" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3298,7 +3337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3514,8 +3553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N160"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView topLeftCell="A131" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3578,8 +3617,8 @@
       <c r="B2" s="3">
         <v>2016</v>
       </c>
-      <c r="C2" s="4">
-        <v>119</v>
+      <c r="C2" s="19">
+        <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>12</v>
@@ -3620,8 +3659,8 @@
       <c r="B3" s="3">
         <v>2016</v>
       </c>
-      <c r="C3" s="4">
-        <v>118</v>
+      <c r="C3" s="20">
+        <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>19</v>
@@ -3662,8 +3701,8 @@
       <c r="B4" s="3">
         <v>2016</v>
       </c>
-      <c r="C4" s="4">
-        <v>112</v>
+      <c r="C4" s="20">
+        <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>25</v>
@@ -3704,8 +3743,8 @@
       <c r="B5" s="3">
         <v>2016</v>
       </c>
-      <c r="C5" s="4">
-        <v>108</v>
+      <c r="C5" s="20">
+        <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>32</v>
@@ -3746,8 +3785,8 @@
       <c r="B6" s="3">
         <v>2016</v>
       </c>
-      <c r="C6" s="4">
-        <v>105</v>
+      <c r="C6" s="20">
+        <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>38</v>
@@ -3788,8 +3827,8 @@
       <c r="B7" s="3">
         <v>2016</v>
       </c>
-      <c r="C7" s="4">
-        <v>104</v>
+      <c r="C7" s="20">
+        <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>44</v>
@@ -3830,8 +3869,8 @@
       <c r="B8" s="3">
         <v>2016</v>
       </c>
-      <c r="C8" s="4">
-        <v>103</v>
+      <c r="C8" s="20">
+        <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>51</v>
@@ -3872,8 +3911,8 @@
       <c r="B9" s="3">
         <v>2016</v>
       </c>
-      <c r="C9" s="4">
-        <v>102</v>
+      <c r="C9" s="20">
+        <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>57</v>
@@ -3914,8 +3953,8 @@
       <c r="B10" s="3">
         <v>2016</v>
       </c>
-      <c r="C10" s="4">
-        <v>101</v>
+      <c r="C10" s="20">
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>61</v>
@@ -3956,8 +3995,8 @@
       <c r="B11" s="3">
         <v>2016</v>
       </c>
-      <c r="C11" s="4">
-        <v>100</v>
+      <c r="C11" s="20">
+        <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>68</v>
@@ -3998,8 +4037,8 @@
       <c r="B12" s="3">
         <v>2016</v>
       </c>
-      <c r="C12" s="4">
-        <v>99</v>
+      <c r="C12" s="20">
+        <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>74</v>
@@ -4040,8 +4079,8 @@
       <c r="B13" s="3">
         <v>2016</v>
       </c>
-      <c r="C13" s="4">
-        <v>97</v>
+      <c r="C13" s="20">
+        <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>81</v>
@@ -4082,8 +4121,8 @@
       <c r="B14" s="3">
         <v>2016</v>
       </c>
-      <c r="C14" s="4">
-        <v>95</v>
+      <c r="C14" s="20">
+        <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>87</v>
@@ -4124,8 +4163,8 @@
       <c r="B15" s="3">
         <v>2016</v>
       </c>
-      <c r="C15" s="4">
-        <v>81</v>
+      <c r="C15" s="20">
+        <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>90</v>
@@ -4166,8 +4205,8 @@
       <c r="B16" s="3">
         <v>2016</v>
       </c>
-      <c r="C16" s="4">
-        <v>78</v>
+      <c r="C16" s="20">
+        <v>15</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>96</v>
@@ -4208,8 +4247,8 @@
       <c r="B17" s="3">
         <v>2016</v>
       </c>
-      <c r="C17" s="4">
-        <v>4</v>
+      <c r="C17" s="20">
+        <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>98</v>
@@ -4250,8 +4289,8 @@
       <c r="B18" s="3">
         <v>2015</v>
       </c>
-      <c r="C18" s="4">
-        <v>3</v>
+      <c r="C18" s="20">
+        <v>17</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>105</v>
@@ -4292,8 +4331,8 @@
       <c r="B19" s="3">
         <v>2015</v>
       </c>
-      <c r="C19" s="4">
-        <v>32</v>
+      <c r="C19" s="20">
+        <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>108</v>
@@ -4334,8 +4373,8 @@
       <c r="B20" s="3">
         <v>2015</v>
       </c>
-      <c r="C20" s="4">
-        <v>40</v>
+      <c r="C20" s="20">
+        <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>114</v>
@@ -4376,8 +4415,8 @@
       <c r="B21" s="3">
         <v>2015</v>
       </c>
-      <c r="C21" s="4">
-        <v>42</v>
+      <c r="C21" s="20">
+        <v>20</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>120</v>
@@ -4418,8 +4457,8 @@
       <c r="B22" s="3">
         <v>2015</v>
       </c>
-      <c r="C22" s="4">
-        <v>66</v>
+      <c r="C22" s="20">
+        <v>21</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>126</v>
@@ -4460,8 +4499,8 @@
       <c r="B23" s="3">
         <v>2015</v>
       </c>
-      <c r="C23" s="4">
-        <v>67</v>
+      <c r="C23" s="20">
+        <v>22</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>132</v>
@@ -4502,8 +4541,8 @@
       <c r="B24" s="3">
         <v>2015</v>
       </c>
-      <c r="C24" s="4">
-        <v>76</v>
+      <c r="C24" s="20">
+        <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>138</v>
@@ -4544,8 +4583,8 @@
       <c r="B25" s="3">
         <v>2015</v>
       </c>
-      <c r="C25" s="4">
-        <v>77</v>
+      <c r="C25" s="20">
+        <v>24</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>144</v>
@@ -4586,8 +4625,8 @@
       <c r="B26" s="3">
         <v>2015</v>
       </c>
-      <c r="C26" s="4">
-        <v>78</v>
+      <c r="C26" s="20">
+        <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>150</v>
@@ -4628,8 +4667,8 @@
       <c r="B27" s="3">
         <v>2015</v>
       </c>
-      <c r="C27" s="4">
-        <v>79</v>
+      <c r="C27" s="20">
+        <v>26</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>156</v>
@@ -4670,8 +4709,8 @@
       <c r="B28" s="3">
         <v>2015</v>
       </c>
-      <c r="C28" s="4">
-        <v>80</v>
+      <c r="C28" s="20">
+        <v>27</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>162</v>
@@ -4712,8 +4751,8 @@
       <c r="B29" s="3">
         <v>2015</v>
       </c>
-      <c r="C29" s="4">
-        <v>81</v>
+      <c r="C29" s="20">
+        <v>28</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>168</v>
@@ -4754,8 +4793,8 @@
       <c r="B30" s="3">
         <v>2015</v>
       </c>
-      <c r="C30" s="4">
-        <v>82</v>
+      <c r="C30" s="20">
+        <v>29</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>174</v>
@@ -4796,8 +4835,8 @@
       <c r="B31" s="3">
         <v>2015</v>
       </c>
-      <c r="C31" s="4">
-        <v>83</v>
+      <c r="C31" s="20">
+        <v>30</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>180</v>
@@ -4838,8 +4877,8 @@
       <c r="B32" s="3">
         <v>2015</v>
       </c>
-      <c r="C32" s="4">
-        <v>84</v>
+      <c r="C32" s="20">
+        <v>31</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>186</v>
@@ -4880,8 +4919,8 @@
       <c r="B33" s="3">
         <v>2015</v>
       </c>
-      <c r="C33" s="4">
-        <v>85</v>
+      <c r="C33" s="20">
+        <v>32</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>192</v>
@@ -4922,8 +4961,8 @@
       <c r="B34" s="3">
         <v>2015</v>
       </c>
-      <c r="C34" s="4">
-        <v>86</v>
+      <c r="C34" s="20">
+        <v>33</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>198</v>
@@ -4964,8 +5003,8 @@
       <c r="B35" s="3">
         <v>2015</v>
       </c>
-      <c r="C35" s="4">
-        <v>87</v>
+      <c r="C35" s="20">
+        <v>34</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>204</v>
@@ -5006,8 +5045,8 @@
       <c r="B36" s="3">
         <v>2015</v>
       </c>
-      <c r="C36" s="4">
-        <v>88</v>
+      <c r="C36" s="20">
+        <v>35</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>210</v>
@@ -5048,8 +5087,8 @@
       <c r="B37" s="3">
         <v>2015</v>
       </c>
-      <c r="C37" s="4">
-        <v>89</v>
+      <c r="C37" s="20">
+        <v>36</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>216</v>
@@ -5090,8 +5129,8 @@
       <c r="B38" s="3">
         <v>2015</v>
       </c>
-      <c r="C38" s="4">
-        <v>90</v>
+      <c r="C38" s="20">
+        <v>37</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>222</v>
@@ -5132,8 +5171,8 @@
       <c r="B39" s="3">
         <v>2015</v>
       </c>
-      <c r="C39" s="4">
-        <v>91</v>
+      <c r="C39" s="20">
+        <v>38</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>224</v>
@@ -5174,8 +5213,8 @@
       <c r="B40" s="3">
         <v>2015</v>
       </c>
-      <c r="C40" s="4">
-        <v>92</v>
+      <c r="C40" s="20">
+        <v>39</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>230</v>
@@ -5216,8 +5255,8 @@
       <c r="B41" s="3">
         <v>2015</v>
       </c>
-      <c r="C41" s="4">
-        <v>93</v>
+      <c r="C41" s="20">
+        <v>40</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>236</v>
@@ -5258,8 +5297,8 @@
       <c r="B42" s="3">
         <v>2015</v>
       </c>
-      <c r="C42" s="4">
-        <v>94</v>
+      <c r="C42" s="20">
+        <v>41</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>242</v>
@@ -5300,8 +5339,8 @@
       <c r="B43" s="3">
         <v>2015</v>
       </c>
-      <c r="C43" s="4">
-        <v>95</v>
+      <c r="C43" s="20">
+        <v>42</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>248</v>
@@ -5342,8 +5381,8 @@
       <c r="B44" s="3">
         <v>2015</v>
       </c>
-      <c r="C44" s="4">
-        <v>96</v>
+      <c r="C44" s="20">
+        <v>43</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>254</v>
@@ -5384,8 +5423,8 @@
       <c r="B45" s="3">
         <v>2015</v>
       </c>
-      <c r="C45" s="4">
-        <v>97</v>
+      <c r="C45" s="20">
+        <v>44</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>260</v>
@@ -5426,8 +5465,8 @@
       <c r="B46" s="3">
         <v>2015</v>
       </c>
-      <c r="C46" s="4">
-        <v>98</v>
+      <c r="C46" s="20">
+        <v>45</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>267</v>
@@ -5468,8 +5507,8 @@
       <c r="B47" s="3">
         <v>2015</v>
       </c>
-      <c r="C47" s="4">
-        <v>99</v>
+      <c r="C47" s="20">
+        <v>46</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>273</v>
@@ -5510,8 +5549,8 @@
       <c r="B48" s="3">
         <v>2015</v>
       </c>
-      <c r="C48" s="4">
-        <v>100</v>
+      <c r="C48" s="20">
+        <v>47</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>279</v>
@@ -5552,8 +5591,8 @@
       <c r="B49" s="3">
         <v>2015</v>
       </c>
-      <c r="C49" s="4">
-        <v>104</v>
+      <c r="C49" s="20">
+        <v>48</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>285</v>
@@ -5594,8 +5633,8 @@
       <c r="B50" s="3">
         <v>2015</v>
       </c>
-      <c r="C50" s="4">
-        <v>1</v>
+      <c r="C50" s="20">
+        <v>49</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>292</v>
@@ -5636,8 +5675,8 @@
       <c r="B51" s="3">
         <v>2015</v>
       </c>
-      <c r="C51" s="4">
-        <v>2</v>
+      <c r="C51" s="20">
+        <v>50</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>298</v>
@@ -5678,8 +5717,8 @@
       <c r="B52" s="3">
         <v>2015</v>
       </c>
-      <c r="C52" s="4">
-        <v>3</v>
+      <c r="C52" s="20">
+        <v>51</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>304</v>
@@ -5720,8 +5759,8 @@
       <c r="B53" s="3">
         <v>2015</v>
       </c>
-      <c r="C53" s="4">
-        <v>4</v>
+      <c r="C53" s="20">
+        <v>52</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>310</v>
@@ -5762,8 +5801,8 @@
       <c r="B54" s="3">
         <v>2015</v>
       </c>
-      <c r="C54" s="4">
-        <v>5</v>
+      <c r="C54" s="20">
+        <v>53</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>316</v>
@@ -5804,8 +5843,8 @@
       <c r="B55" s="3">
         <v>2015</v>
       </c>
-      <c r="C55" s="4">
-        <v>13</v>
+      <c r="C55" s="20">
+        <v>54</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>322</v>
@@ -5846,8 +5885,8 @@
       <c r="B56" s="3">
         <v>2015</v>
       </c>
-      <c r="C56" s="4">
-        <v>96</v>
+      <c r="C56" s="20">
+        <v>55</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>328</v>
@@ -5888,8 +5927,8 @@
       <c r="B57" s="3">
         <v>2015</v>
       </c>
-      <c r="C57" s="4">
-        <v>97</v>
+      <c r="C57" s="20">
+        <v>56</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>334</v>
@@ -5930,8 +5969,8 @@
       <c r="B58" s="3">
         <v>2015</v>
       </c>
-      <c r="C58" s="4">
-        <v>98</v>
+      <c r="C58" s="20">
+        <v>57</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>340</v>
@@ -5972,8 +6011,8 @@
       <c r="B59" s="3">
         <v>2015</v>
       </c>
-      <c r="C59" s="4">
-        <v>99</v>
+      <c r="C59" s="20">
+        <v>58</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>346</v>
@@ -6014,8 +6053,8 @@
       <c r="B60" s="3">
         <v>2015</v>
       </c>
-      <c r="C60" s="4">
-        <v>100</v>
+      <c r="C60" s="20">
+        <v>59</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>352</v>
@@ -6056,8 +6095,8 @@
       <c r="B61" s="3">
         <v>2015</v>
       </c>
-      <c r="C61" s="4">
-        <v>102</v>
+      <c r="C61" s="20">
+        <v>60</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>358</v>
@@ -6098,8 +6137,8 @@
       <c r="B62" s="3">
         <v>2015</v>
       </c>
-      <c r="C62" s="4">
-        <v>103</v>
+      <c r="C62" s="20">
+        <v>61</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>364</v>
@@ -6140,8 +6179,8 @@
       <c r="B63" s="3">
         <v>2015</v>
       </c>
-      <c r="C63" s="4">
-        <v>104</v>
+      <c r="C63" s="20">
+        <v>62</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>370</v>
@@ -6182,8 +6221,8 @@
       <c r="B64" s="3">
         <v>2015</v>
       </c>
-      <c r="C64" s="4">
-        <v>105</v>
+      <c r="C64" s="20">
+        <v>63</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>376</v>
@@ -6224,8 +6263,8 @@
       <c r="B65" s="3">
         <v>2015</v>
       </c>
-      <c r="C65" s="4">
-        <v>106</v>
+      <c r="C65" s="20">
+        <v>64</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>376</v>
@@ -6266,8 +6305,8 @@
       <c r="B66" s="3">
         <v>2015</v>
       </c>
-      <c r="C66" s="4">
-        <v>109</v>
+      <c r="C66" s="20">
+        <v>65</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>387</v>
@@ -6308,8 +6347,8 @@
       <c r="B67" s="3">
         <v>2015</v>
       </c>
-      <c r="C67" s="4">
-        <v>110</v>
+      <c r="C67" s="20">
+        <v>66</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>393</v>
@@ -6350,8 +6389,8 @@
       <c r="B68" s="3">
         <v>2015</v>
       </c>
-      <c r="C68" s="4">
-        <v>111</v>
+      <c r="C68" s="20">
+        <v>67</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>399</v>
@@ -6392,8 +6431,8 @@
       <c r="B69" s="3">
         <v>2015</v>
       </c>
-      <c r="C69" s="4">
-        <v>112</v>
+      <c r="C69" s="20">
+        <v>68</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>376</v>
@@ -6434,8 +6473,8 @@
       <c r="B70" s="3">
         <v>2015</v>
       </c>
-      <c r="C70" s="4">
-        <v>113</v>
+      <c r="C70" s="20">
+        <v>69</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>410</v>
@@ -6476,8 +6515,8 @@
       <c r="B71" s="3">
         <v>2015</v>
       </c>
-      <c r="C71" s="4">
-        <v>115</v>
+      <c r="C71" s="20">
+        <v>70</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>416</v>
@@ -6518,8 +6557,8 @@
       <c r="B72" s="3">
         <v>2015</v>
       </c>
-      <c r="C72" s="4">
-        <v>116</v>
+      <c r="C72" s="20">
+        <v>71</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>376</v>
@@ -6560,8 +6599,8 @@
       <c r="B73" s="3">
         <v>2015</v>
       </c>
-      <c r="C73" s="4">
-        <v>117</v>
+      <c r="C73" s="20">
+        <v>72</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>376</v>
@@ -6602,8 +6641,8 @@
       <c r="B74" s="3">
         <v>2015</v>
       </c>
-      <c r="C74" s="4">
-        <v>119</v>
+      <c r="C74" s="20">
+        <v>73</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>432</v>
@@ -6644,8 +6683,8 @@
       <c r="B75" s="3">
         <v>2015</v>
       </c>
-      <c r="C75" s="4">
-        <v>8</v>
+      <c r="C75" s="20">
+        <v>74</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>439</v>
@@ -6686,8 +6725,8 @@
       <c r="B76" s="3">
         <v>2015</v>
       </c>
-      <c r="C76" s="4">
-        <v>13</v>
+      <c r="C76" s="20">
+        <v>75</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>445</v>
@@ -6728,8 +6767,8 @@
       <c r="B77" s="3">
         <v>2015</v>
       </c>
-      <c r="C77" s="4">
-        <v>17</v>
+      <c r="C77" s="20">
+        <v>76</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>451</v>
@@ -6770,8 +6809,8 @@
       <c r="B78" s="3">
         <v>2015</v>
       </c>
-      <c r="C78" s="4">
-        <v>19</v>
+      <c r="C78" s="20">
+        <v>77</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>457</v>
@@ -6812,8 +6851,8 @@
       <c r="B79" s="3">
         <v>2015</v>
       </c>
-      <c r="C79" s="4">
-        <v>24</v>
+      <c r="C79" s="20">
+        <v>78</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>463</v>
@@ -6854,8 +6893,8 @@
       <c r="B80" s="3">
         <v>2015</v>
       </c>
-      <c r="C80" s="4">
-        <v>37</v>
+      <c r="C80" s="20">
+        <v>79</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>465</v>
@@ -6896,8 +6935,8 @@
       <c r="B81" s="3">
         <v>2015</v>
       </c>
-      <c r="C81" s="4">
-        <v>39</v>
+      <c r="C81" s="20">
+        <v>80</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>471</v>
@@ -6938,8 +6977,8 @@
       <c r="B82" s="3">
         <v>2015</v>
       </c>
-      <c r="C82" s="4">
-        <v>41</v>
+      <c r="C82" s="20">
+        <v>81</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>477</v>
@@ -6980,8 +7019,8 @@
       <c r="B83" s="3">
         <v>2015</v>
       </c>
-      <c r="C83" s="4">
-        <v>42</v>
+      <c r="C83" s="20">
+        <v>82</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>483</v>
@@ -7022,8 +7061,8 @@
       <c r="B84" s="3">
         <v>2015</v>
       </c>
-      <c r="C84" s="4">
-        <v>43</v>
+      <c r="C84" s="20">
+        <v>83</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>485</v>
@@ -7064,8 +7103,8 @@
       <c r="B85" s="3">
         <v>2015</v>
       </c>
-      <c r="C85" s="4">
-        <v>52</v>
+      <c r="C85" s="20">
+        <v>84</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>491</v>
@@ -7106,8 +7145,8 @@
       <c r="B86" s="3">
         <v>2015</v>
       </c>
-      <c r="C86" s="4">
-        <v>53</v>
+      <c r="C86" s="20">
+        <v>85</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>497</v>
@@ -7148,8 +7187,8 @@
       <c r="B87" s="3">
         <v>2015</v>
       </c>
-      <c r="C87" s="4">
-        <v>63</v>
+      <c r="C87" s="20">
+        <v>86</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>502</v>
@@ -7190,8 +7229,8 @@
       <c r="B88" s="3">
         <v>2015</v>
       </c>
-      <c r="C88" s="4">
-        <v>65</v>
+      <c r="C88" s="20">
+        <v>87</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>508</v>
@@ -7232,8 +7271,8 @@
       <c r="B89" s="3">
         <v>2015</v>
       </c>
-      <c r="C89" s="4">
-        <v>7</v>
+      <c r="C89" s="20">
+        <v>88</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>514</v>
@@ -7274,8 +7313,8 @@
       <c r="B90" s="3">
         <v>2015</v>
       </c>
-      <c r="C90" s="4">
-        <v>69</v>
+      <c r="C90" s="20">
+        <v>89</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>520</v>
@@ -7316,8 +7355,8 @@
       <c r="B91" s="3">
         <v>2015</v>
       </c>
-      <c r="C91" s="4">
-        <v>91</v>
+      <c r="C91" s="20">
+        <v>90</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>526</v>
@@ -7358,8 +7397,8 @@
       <c r="B92" s="3">
         <v>2015</v>
       </c>
-      <c r="C92" s="4">
-        <v>92</v>
+      <c r="C92" s="20">
+        <v>91</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>532</v>
@@ -7400,8 +7439,8 @@
       <c r="B93" s="3">
         <v>2015</v>
       </c>
-      <c r="C93" s="4">
-        <v>93</v>
+      <c r="C93" s="20">
+        <v>92</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>538</v>
@@ -7442,8 +7481,8 @@
       <c r="B94" s="3">
         <v>2015</v>
       </c>
-      <c r="C94" s="4">
-        <v>96</v>
+      <c r="C94" s="20">
+        <v>93</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>544</v>
@@ -7484,8 +7523,8 @@
       <c r="B95" s="3">
         <v>2015</v>
       </c>
-      <c r="C95" s="4">
-        <v>99</v>
+      <c r="C95" s="20">
+        <v>94</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>550</v>
@@ -7526,8 +7565,8 @@
       <c r="B96" s="3">
         <v>2015</v>
       </c>
-      <c r="C96" s="4">
-        <v>113</v>
+      <c r="C96" s="20">
+        <v>95</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>556</v>
@@ -7568,8 +7607,8 @@
       <c r="B97" s="3">
         <v>2015</v>
       </c>
-      <c r="C97" s="4">
-        <v>1</v>
+      <c r="C97" s="20">
+        <v>96</v>
       </c>
       <c r="D97" s="7" t="s">
         <v>563</v>
@@ -7610,8 +7649,8 @@
       <c r="B98" s="3">
         <v>2015</v>
       </c>
-      <c r="C98" s="4">
-        <v>2</v>
+      <c r="C98" s="20">
+        <v>97</v>
       </c>
       <c r="D98" s="7" t="s">
         <v>569</v>
@@ -7652,8 +7691,8 @@
       <c r="B99" s="3">
         <v>2015</v>
       </c>
-      <c r="C99" s="4">
-        <v>3</v>
+      <c r="C99" s="20">
+        <v>98</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>575</v>
@@ -7694,8 +7733,8 @@
       <c r="B100" s="3">
         <v>2015</v>
       </c>
-      <c r="C100" s="4">
-        <v>4</v>
+      <c r="C100" s="20">
+        <v>99</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>581</v>
@@ -7736,8 +7775,8 @@
       <c r="B101" s="3">
         <v>2015</v>
       </c>
-      <c r="C101" s="4">
-        <v>5</v>
+      <c r="C101" s="20">
+        <v>100</v>
       </c>
       <c r="D101" s="7" t="s">
         <v>587</v>
@@ -7778,8 +7817,8 @@
       <c r="B102" s="3">
         <v>2015</v>
       </c>
-      <c r="C102" s="4">
-        <v>6</v>
+      <c r="C102" s="20">
+        <v>101</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>593</v>
@@ -7820,8 +7859,8 @@
       <c r="B103" s="3">
         <v>2015</v>
       </c>
-      <c r="C103" s="4">
-        <v>7</v>
+      <c r="C103" s="20">
+        <v>102</v>
       </c>
       <c r="D103" s="7" t="s">
         <v>599</v>
@@ -7862,8 +7901,8 @@
       <c r="B104" s="3">
         <v>2015</v>
       </c>
-      <c r="C104" s="4">
-        <v>8</v>
+      <c r="C104" s="20">
+        <v>103</v>
       </c>
       <c r="D104" s="7" t="s">
         <v>605</v>
@@ -7904,8 +7943,8 @@
       <c r="B105" s="3">
         <v>2015</v>
       </c>
-      <c r="C105" s="4">
-        <v>9</v>
+      <c r="C105" s="20">
+        <v>104</v>
       </c>
       <c r="D105" s="7" t="s">
         <v>611</v>
@@ -7946,8 +7985,8 @@
       <c r="B106" s="3">
         <v>2015</v>
       </c>
-      <c r="C106" s="4">
-        <v>10</v>
+      <c r="C106" s="20">
+        <v>105</v>
       </c>
       <c r="D106" s="7" t="s">
         <v>617</v>
@@ -7988,8 +8027,8 @@
       <c r="B107" s="3">
         <v>2015</v>
       </c>
-      <c r="C107" s="4">
-        <v>11</v>
+      <c r="C107" s="20">
+        <v>106</v>
       </c>
       <c r="D107" s="7" t="s">
         <v>623</v>
@@ -8030,8 +8069,8 @@
       <c r="B108" s="3">
         <v>2015</v>
       </c>
-      <c r="C108" s="4">
-        <v>12</v>
+      <c r="C108" s="20">
+        <v>107</v>
       </c>
       <c r="D108" s="7" t="s">
         <v>629</v>
@@ -8072,8 +8111,8 @@
       <c r="B109" s="3">
         <v>2015</v>
       </c>
-      <c r="C109" s="4">
-        <v>112</v>
+      <c r="C109" s="20">
+        <v>108</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>636</v>
@@ -8114,8 +8153,8 @@
       <c r="B110" s="3">
         <v>2015</v>
       </c>
-      <c r="C110" s="4">
-        <v>54</v>
+      <c r="C110" s="20">
+        <v>109</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>643</v>
@@ -8156,8 +8195,8 @@
       <c r="B111" s="3">
         <v>2015</v>
       </c>
-      <c r="C111" s="4">
-        <v>55</v>
+      <c r="C111" s="20">
+        <v>110</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>649</v>
@@ -8198,8 +8237,8 @@
       <c r="B112" s="3">
         <v>2015</v>
       </c>
-      <c r="C112" s="4">
-        <v>56</v>
+      <c r="C112" s="20">
+        <v>111</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>655</v>
@@ -8240,8 +8279,8 @@
       <c r="B113" s="3">
         <v>2015</v>
       </c>
-      <c r="C113" s="4">
-        <v>57</v>
+      <c r="C113" s="20">
+        <v>112</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>661</v>
@@ -8282,8 +8321,8 @@
       <c r="B114" s="3">
         <v>2015</v>
       </c>
-      <c r="C114" s="4">
-        <v>58</v>
+      <c r="C114" s="20">
+        <v>113</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>667</v>
@@ -8324,8 +8363,8 @@
       <c r="B115" s="3">
         <v>2015</v>
       </c>
-      <c r="C115" s="4">
-        <v>59</v>
+      <c r="C115" s="20">
+        <v>114</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>673</v>
@@ -8366,8 +8405,8 @@
       <c r="B116" s="3">
         <v>2015</v>
       </c>
-      <c r="C116" s="4">
-        <v>60</v>
+      <c r="C116" s="20">
+        <v>115</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>679</v>
@@ -8408,8 +8447,8 @@
       <c r="B117" s="3">
         <v>2015</v>
       </c>
-      <c r="C117" s="4">
-        <v>61</v>
+      <c r="C117" s="20">
+        <v>116</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>685</v>
@@ -8450,8 +8489,8 @@
       <c r="B118" s="3">
         <v>2015</v>
       </c>
-      <c r="C118" s="4">
-        <v>62</v>
+      <c r="C118" s="20">
+        <v>117</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>691</v>
@@ -8492,8 +8531,8 @@
       <c r="B119" s="3">
         <v>2015</v>
       </c>
-      <c r="C119" s="4">
-        <v>63</v>
+      <c r="C119" s="20">
+        <v>118</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>697</v>
@@ -8534,8 +8573,8 @@
       <c r="B120" s="3">
         <v>2015</v>
       </c>
-      <c r="C120" s="4">
-        <v>64</v>
+      <c r="C120" s="20">
+        <v>119</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>703</v>
@@ -8576,8 +8615,8 @@
       <c r="B121" s="3">
         <v>2015</v>
       </c>
-      <c r="C121" s="4">
-        <v>65</v>
+      <c r="C121" s="20">
+        <v>120</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>709</v>
@@ -8618,8 +8657,8 @@
       <c r="B122" s="3">
         <v>2015</v>
       </c>
-      <c r="C122" s="4">
-        <v>81</v>
+      <c r="C122" s="20">
+        <v>121</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>715</v>
@@ -8660,8 +8699,8 @@
       <c r="B123" s="3">
         <v>2015</v>
       </c>
-      <c r="C123" s="4">
-        <v>82</v>
+      <c r="C123" s="20">
+        <v>122</v>
       </c>
       <c r="D123" s="5" t="s">
         <v>376</v>
@@ -8702,8 +8741,8 @@
       <c r="B124" s="3">
         <v>2015</v>
       </c>
-      <c r="C124" s="4">
-        <v>83</v>
+      <c r="C124" s="20">
+        <v>123</v>
       </c>
       <c r="D124" s="5" t="s">
         <v>726</v>
@@ -8744,8 +8783,8 @@
       <c r="B125" s="3">
         <v>2015</v>
       </c>
-      <c r="C125" s="4">
-        <v>84</v>
+      <c r="C125" s="20">
+        <v>124</v>
       </c>
       <c r="D125" s="5" t="s">
         <v>358</v>
@@ -8786,8 +8825,8 @@
       <c r="B126" s="3">
         <v>2015</v>
       </c>
-      <c r="C126" s="4">
-        <v>85</v>
+      <c r="C126" s="20">
+        <v>125</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>737</v>
@@ -8828,8 +8867,8 @@
       <c r="B127" s="3">
         <v>2015</v>
       </c>
-      <c r="C127" s="4">
-        <v>86</v>
+      <c r="C127" s="20">
+        <v>126</v>
       </c>
       <c r="D127" s="5" t="s">
         <v>743</v>
@@ -8870,8 +8909,8 @@
       <c r="B128" s="3">
         <v>2015</v>
       </c>
-      <c r="C128" s="4">
-        <v>87</v>
+      <c r="C128" s="20">
+        <v>127</v>
       </c>
       <c r="D128" s="5" t="s">
         <v>748</v>
@@ -8912,8 +8951,8 @@
       <c r="B129" s="3">
         <v>2015</v>
       </c>
-      <c r="C129" s="4">
-        <v>88</v>
+      <c r="C129" s="20">
+        <v>128</v>
       </c>
       <c r="D129" s="5" t="s">
         <v>754</v>
@@ -8954,8 +8993,8 @@
       <c r="B130" s="3">
         <v>2015</v>
       </c>
-      <c r="C130" s="4">
-        <v>89</v>
+      <c r="C130" s="20">
+        <v>129</v>
       </c>
       <c r="D130" s="5" t="s">
         <v>760</v>
@@ -8996,8 +9035,8 @@
       <c r="B131" s="3">
         <v>2015</v>
       </c>
-      <c r="C131" s="4">
-        <v>90</v>
+      <c r="C131" s="20">
+        <v>130</v>
       </c>
       <c r="D131" s="5" t="s">
         <v>766</v>
@@ -9038,8 +9077,8 @@
       <c r="B132" s="3">
         <v>2015</v>
       </c>
-      <c r="C132" s="4">
-        <v>91</v>
+      <c r="C132" s="20">
+        <v>131</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>772</v>
@@ -9080,8 +9119,8 @@
       <c r="B133" s="3">
         <v>2015</v>
       </c>
-      <c r="C133" s="4">
-        <v>92</v>
+      <c r="C133" s="20">
+        <v>132</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>778</v>
@@ -9122,8 +9161,8 @@
       <c r="B134" s="3">
         <v>2015</v>
       </c>
-      <c r="C134" s="4">
-        <v>93</v>
+      <c r="C134" s="20">
+        <v>133</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>784</v>
@@ -9164,8 +9203,8 @@
       <c r="B135" s="3">
         <v>2015</v>
       </c>
-      <c r="C135" s="4">
-        <v>94</v>
+      <c r="C135" s="20">
+        <v>134</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>790</v>
@@ -9206,8 +9245,8 @@
       <c r="B136" s="3">
         <v>2015</v>
       </c>
-      <c r="C136" s="4">
-        <v>95</v>
+      <c r="C136" s="20">
+        <v>135</v>
       </c>
       <c r="D136" s="5" t="s">
         <v>796</v>
@@ -9248,8 +9287,8 @@
       <c r="B137" s="3">
         <v>2015</v>
       </c>
-      <c r="C137" s="4">
-        <v>96</v>
+      <c r="C137" s="20">
+        <v>136</v>
       </c>
       <c r="D137" s="5" t="s">
         <v>801</v>
@@ -9290,8 +9329,8 @@
       <c r="B138" s="3">
         <v>2015</v>
       </c>
-      <c r="C138" s="4">
-        <v>97</v>
+      <c r="C138" s="20">
+        <v>137</v>
       </c>
       <c r="D138" s="5" t="s">
         <v>807</v>
@@ -9332,8 +9371,8 @@
       <c r="B139" s="3">
         <v>2015</v>
       </c>
-      <c r="C139" s="4">
-        <v>98</v>
+      <c r="C139" s="20">
+        <v>138</v>
       </c>
       <c r="D139" s="5" t="s">
         <v>813</v>
@@ -9374,8 +9413,8 @@
       <c r="B140" s="3">
         <v>2015</v>
       </c>
-      <c r="C140" s="4">
-        <v>99</v>
+      <c r="C140" s="20">
+        <v>139</v>
       </c>
       <c r="D140" s="5" t="s">
         <v>819</v>
@@ -9416,8 +9455,8 @@
       <c r="B141" s="3">
         <v>2015</v>
       </c>
-      <c r="C141" s="4">
-        <v>100</v>
+      <c r="C141" s="20">
+        <v>140</v>
       </c>
       <c r="D141" s="5" t="s">
         <v>825</v>
@@ -9458,8 +9497,8 @@
       <c r="B142" s="3">
         <v>2015</v>
       </c>
-      <c r="C142" s="4">
-        <v>101</v>
+      <c r="C142" s="20">
+        <v>141</v>
       </c>
       <c r="D142" s="5" t="s">
         <v>831</v>
@@ -9500,8 +9539,8 @@
       <c r="B143" s="3">
         <v>2015</v>
       </c>
-      <c r="C143" s="4">
-        <v>102</v>
+      <c r="C143" s="20">
+        <v>142</v>
       </c>
       <c r="D143" s="5" t="s">
         <v>834</v>
@@ -9542,8 +9581,8 @@
       <c r="B144" s="3">
         <v>2015</v>
       </c>
-      <c r="C144" s="4">
-        <v>103</v>
+      <c r="C144" s="20">
+        <v>143</v>
       </c>
       <c r="D144" s="5" t="s">
         <v>840</v>
@@ -9584,8 +9623,8 @@
       <c r="B145" s="3">
         <v>2015</v>
       </c>
-      <c r="C145" s="4">
-        <v>104</v>
+      <c r="C145" s="20">
+        <v>144</v>
       </c>
       <c r="D145" s="5" t="s">
         <v>845</v>
@@ -9626,8 +9665,8 @@
       <c r="B146" s="3">
         <v>2015</v>
       </c>
-      <c r="C146" s="4">
-        <v>105</v>
+      <c r="C146" s="20">
+        <v>145</v>
       </c>
       <c r="D146" s="5" t="s">
         <v>851</v>
@@ -9668,8 +9707,8 @@
       <c r="B147" s="3">
         <v>2015</v>
       </c>
-      <c r="C147" s="4">
-        <v>106</v>
+      <c r="C147" s="20">
+        <v>146</v>
       </c>
       <c r="D147" s="5" t="s">
         <v>857</v>
@@ -9710,8 +9749,8 @@
       <c r="B148" s="3">
         <v>2015</v>
       </c>
-      <c r="C148" s="4">
-        <v>107</v>
+      <c r="C148" s="20">
+        <v>147</v>
       </c>
       <c r="D148" s="5" t="s">
         <v>863</v>
@@ -9752,8 +9791,8 @@
       <c r="B149" s="3">
         <v>2015</v>
       </c>
-      <c r="C149" s="4">
-        <v>108</v>
+      <c r="C149" s="20">
+        <v>148</v>
       </c>
       <c r="D149" s="5" t="s">
         <v>869</v>
@@ -9794,8 +9833,8 @@
       <c r="B150" s="3">
         <v>2015</v>
       </c>
-      <c r="C150" s="4">
-        <v>109</v>
+      <c r="C150" s="20">
+        <v>149</v>
       </c>
       <c r="D150" s="5" t="s">
         <v>874</v>
@@ -9836,8 +9875,8 @@
       <c r="B151" s="3">
         <v>2015</v>
       </c>
-      <c r="C151" s="4">
-        <v>110</v>
+      <c r="C151" s="20">
+        <v>150</v>
       </c>
       <c r="D151" s="5" t="s">
         <v>880</v>
@@ -9878,8 +9917,8 @@
       <c r="B152" s="3">
         <v>2015</v>
       </c>
-      <c r="C152" s="4">
-        <v>111</v>
+      <c r="C152" s="20">
+        <v>151</v>
       </c>
       <c r="D152" s="5" t="s">
         <v>886</v>
@@ -9920,8 +9959,8 @@
       <c r="B153" s="3">
         <v>2015</v>
       </c>
-      <c r="C153" s="4">
-        <v>112</v>
+      <c r="C153" s="20">
+        <v>152</v>
       </c>
       <c r="D153" s="5" t="s">
         <v>892</v>
@@ -9962,8 +10001,8 @@
       <c r="B154" s="3">
         <v>2015</v>
       </c>
-      <c r="C154" s="4">
-        <v>113</v>
+      <c r="C154" s="20">
+        <v>153</v>
       </c>
       <c r="D154" s="5" t="s">
         <v>894</v>
@@ -10004,8 +10043,8 @@
       <c r="B155" s="3">
         <v>2015</v>
       </c>
-      <c r="C155" s="4">
-        <v>114</v>
+      <c r="C155" s="20">
+        <v>154</v>
       </c>
       <c r="D155" s="5" t="s">
         <v>900</v>
@@ -10046,8 +10085,8 @@
       <c r="B156" s="3">
         <v>2015</v>
       </c>
-      <c r="C156" s="4">
-        <v>115</v>
+      <c r="C156" s="20">
+        <v>155</v>
       </c>
       <c r="D156" s="5" t="s">
         <v>906</v>
@@ -10088,8 +10127,8 @@
       <c r="B157" s="3">
         <v>2015</v>
       </c>
-      <c r="C157" s="4">
-        <v>116</v>
+      <c r="C157" s="20">
+        <v>156</v>
       </c>
       <c r="D157" s="5" t="s">
         <v>912</v>
@@ -10130,8 +10169,8 @@
       <c r="B158" s="3">
         <v>2015</v>
       </c>
-      <c r="C158" s="4">
-        <v>119</v>
+      <c r="C158" s="20">
+        <v>157</v>
       </c>
       <c r="D158" s="5" t="s">
         <v>918</v>
@@ -10181,8 +10220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10251,8 +10290,8 @@
       <c r="B2" s="3">
         <v>2016</v>
       </c>
-      <c r="C2" s="4">
-        <v>101</v>
+      <c r="C2" s="19">
+        <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>61</v>
@@ -10297,8 +10336,8 @@
       <c r="B3" s="3">
         <v>2016</v>
       </c>
-      <c r="C3" s="4">
-        <v>100</v>
+      <c r="C3" s="20">
+        <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>68</v>
@@ -10343,8 +10382,8 @@
       <c r="B4" s="3">
         <v>2016</v>
       </c>
-      <c r="C4" s="4">
-        <v>99</v>
+      <c r="C4" s="20">
+        <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>74</v>
@@ -10389,8 +10428,8 @@
       <c r="B5" s="3">
         <v>2016</v>
       </c>
-      <c r="C5" s="4">
-        <v>97</v>
+      <c r="C5" s="20">
+        <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>81</v>
@@ -10435,8 +10474,8 @@
       <c r="B6" s="3">
         <v>2016</v>
       </c>
-      <c r="C6" s="4">
-        <v>95</v>
+      <c r="C6" s="20">
+        <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>87</v>
@@ -10481,8 +10520,8 @@
       <c r="B7" s="3">
         <v>2016</v>
       </c>
-      <c r="C7" s="4">
-        <v>81</v>
+      <c r="C7" s="20">
+        <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>90</v>
@@ -10527,8 +10566,8 @@
       <c r="B8" s="3">
         <v>2016</v>
       </c>
-      <c r="C8" s="4">
-        <v>78</v>
+      <c r="C8" s="20">
+        <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>96</v>
@@ -10573,8 +10612,8 @@
       <c r="B9" s="3">
         <v>2016</v>
       </c>
-      <c r="C9" s="4">
-        <v>4</v>
+      <c r="C9" s="20">
+        <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>98</v>
@@ -10619,8 +10658,8 @@
       <c r="B10" s="3">
         <v>2015</v>
       </c>
-      <c r="C10" s="4">
-        <v>3</v>
+      <c r="C10" s="20">
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>105</v>
@@ -10665,8 +10704,8 @@
       <c r="B11" s="3">
         <v>2015</v>
       </c>
-      <c r="C11" s="4">
-        <v>32</v>
+      <c r="C11" s="20">
+        <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>108</v>
@@ -10707,8 +10746,8 @@
       <c r="B12" s="3">
         <v>2015</v>
       </c>
-      <c r="C12" s="4">
-        <v>40</v>
+      <c r="C12" s="20">
+        <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>114</v>
@@ -10749,8 +10788,8 @@
       <c r="B13" s="3">
         <v>2015</v>
       </c>
-      <c r="C13" s="4">
-        <v>42</v>
+      <c r="C13" s="20">
+        <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>120</v>
@@ -10791,8 +10830,8 @@
       <c r="B14" s="3">
         <v>2016</v>
       </c>
-      <c r="C14" s="4">
-        <v>119</v>
+      <c r="C14" s="20">
+        <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>12</v>
@@ -10833,8 +10872,8 @@
       <c r="B15" s="3">
         <v>2016</v>
       </c>
-      <c r="C15" s="4">
-        <v>118</v>
+      <c r="C15" s="20">
+        <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>19</v>
@@ -10875,8 +10914,8 @@
       <c r="B16" s="3">
         <v>2016</v>
       </c>
-      <c r="C16" s="4">
-        <v>112</v>
+      <c r="C16" s="20">
+        <v>15</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>25</v>
@@ -10917,8 +10956,8 @@
       <c r="B17" s="3">
         <v>2016</v>
       </c>
-      <c r="C17" s="4">
-        <v>108</v>
+      <c r="C17" s="20">
+        <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>32</v>
@@ -10959,8 +10998,8 @@
       <c r="B18" s="3">
         <v>2016</v>
       </c>
-      <c r="C18" s="4">
-        <v>105</v>
+      <c r="C18" s="20">
+        <v>17</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>38</v>
@@ -11001,8 +11040,8 @@
       <c r="B19" s="3">
         <v>2016</v>
       </c>
-      <c r="C19" s="4">
-        <v>104</v>
+      <c r="C19" s="20">
+        <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>44</v>
@@ -11043,8 +11082,8 @@
       <c r="B20" s="3">
         <v>2016</v>
       </c>
-      <c r="C20" s="4">
-        <v>103</v>
+      <c r="C20" s="20">
+        <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>51</v>
@@ -11085,8 +11124,8 @@
       <c r="B21" s="3">
         <v>2016</v>
       </c>
-      <c r="C21" s="4">
-        <v>102</v>
+      <c r="C21" s="20">
+        <v>20</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>57</v>
@@ -11127,8 +11166,8 @@
       <c r="B22" s="3">
         <v>2015</v>
       </c>
-      <c r="C22" s="4">
-        <v>66</v>
+      <c r="C22" s="20">
+        <v>21</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>126</v>
@@ -11169,8 +11208,8 @@
       <c r="B23" s="3">
         <v>2015</v>
       </c>
-      <c r="C23" s="4">
-        <v>67</v>
+      <c r="C23" s="20">
+        <v>22</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>132</v>
@@ -11211,8 +11250,8 @@
       <c r="B24" s="3">
         <v>2015</v>
       </c>
-      <c r="C24" s="4">
-        <v>76</v>
+      <c r="C24" s="20">
+        <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>138</v>
@@ -11253,8 +11292,8 @@
       <c r="B25" s="3">
         <v>2015</v>
       </c>
-      <c r="C25" s="4">
-        <v>77</v>
+      <c r="C25" s="20">
+        <v>24</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>144</v>
@@ -11295,8 +11334,8 @@
       <c r="B26" s="3">
         <v>2015</v>
       </c>
-      <c r="C26" s="4">
-        <v>78</v>
+      <c r="C26" s="20">
+        <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>150</v>
@@ -11337,8 +11376,8 @@
       <c r="B27" s="3">
         <v>2015</v>
       </c>
-      <c r="C27" s="4">
-        <v>79</v>
+      <c r="C27" s="19">
+        <v>26</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>156</v>
@@ -11379,8 +11418,8 @@
       <c r="B28" s="3">
         <v>2015</v>
       </c>
-      <c r="C28" s="4">
-        <v>80</v>
+      <c r="C28" s="20">
+        <v>27</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>162</v>
@@ -11421,8 +11460,8 @@
       <c r="B29" s="3">
         <v>2015</v>
       </c>
-      <c r="C29" s="4">
-        <v>81</v>
+      <c r="C29" s="20">
+        <v>28</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>168</v>
@@ -11463,8 +11502,8 @@
       <c r="B30" s="3">
         <v>2015</v>
       </c>
-      <c r="C30" s="4">
-        <v>82</v>
+      <c r="C30" s="20">
+        <v>29</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>174</v>
@@ -11505,8 +11544,8 @@
       <c r="B31" s="3">
         <v>2015</v>
       </c>
-      <c r="C31" s="4">
-        <v>83</v>
+      <c r="C31" s="20">
+        <v>30</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>180</v>
@@ -11547,8 +11586,8 @@
       <c r="B32" s="3">
         <v>2015</v>
       </c>
-      <c r="C32" s="4">
-        <v>84</v>
+      <c r="C32" s="20">
+        <v>31</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>186</v>
@@ -11589,8 +11628,8 @@
       <c r="B33" s="3">
         <v>2015</v>
       </c>
-      <c r="C33" s="4">
-        <v>85</v>
+      <c r="C33" s="20">
+        <v>32</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>192</v>
@@ -11631,8 +11670,8 @@
       <c r="B34" s="3">
         <v>2015</v>
       </c>
-      <c r="C34" s="4">
-        <v>86</v>
+      <c r="C34" s="20">
+        <v>33</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>198</v>
@@ -11673,8 +11712,8 @@
       <c r="B35" s="3">
         <v>2015</v>
       </c>
-      <c r="C35" s="4">
-        <v>87</v>
+      <c r="C35" s="20">
+        <v>34</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>204</v>
@@ -11715,8 +11754,8 @@
       <c r="B36" s="3">
         <v>2015</v>
       </c>
-      <c r="C36" s="4">
-        <v>88</v>
+      <c r="C36" s="20">
+        <v>35</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>210</v>
@@ -11757,8 +11796,8 @@
       <c r="B37" s="3">
         <v>2015</v>
       </c>
-      <c r="C37" s="4">
-        <v>89</v>
+      <c r="C37" s="20">
+        <v>36</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>216</v>
@@ -11799,8 +11838,8 @@
       <c r="B38" s="3">
         <v>2015</v>
       </c>
-      <c r="C38" s="4">
-        <v>90</v>
+      <c r="C38" s="20">
+        <v>37</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>222</v>
@@ -11841,8 +11880,8 @@
       <c r="B39" s="3">
         <v>2015</v>
       </c>
-      <c r="C39" s="4">
-        <v>91</v>
+      <c r="C39" s="20">
+        <v>38</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>224</v>
@@ -11883,8 +11922,8 @@
       <c r="B40" s="3">
         <v>2015</v>
       </c>
-      <c r="C40" s="4">
-        <v>92</v>
+      <c r="C40" s="20">
+        <v>39</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>230</v>
@@ -11925,8 +11964,8 @@
       <c r="B41" s="3">
         <v>2015</v>
       </c>
-      <c r="C41" s="4">
-        <v>93</v>
+      <c r="C41" s="20">
+        <v>40</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>236</v>
@@ -11967,8 +12006,8 @@
       <c r="B42" s="3">
         <v>2015</v>
       </c>
-      <c r="C42" s="4">
-        <v>94</v>
+      <c r="C42" s="20">
+        <v>41</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>242</v>
@@ -12009,8 +12048,8 @@
       <c r="B43" s="3">
         <v>2015</v>
       </c>
-      <c r="C43" s="4">
-        <v>95</v>
+      <c r="C43" s="20">
+        <v>42</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>248</v>
@@ -12051,8 +12090,8 @@
       <c r="B44" s="3">
         <v>2015</v>
       </c>
-      <c r="C44" s="4">
-        <v>96</v>
+      <c r="C44" s="20">
+        <v>43</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>254</v>
@@ -12093,8 +12132,8 @@
       <c r="B45" s="3">
         <v>2015</v>
       </c>
-      <c r="C45" s="4">
-        <v>97</v>
+      <c r="C45" s="20">
+        <v>44</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>260</v>
@@ -12135,8 +12174,8 @@
       <c r="B46" s="3">
         <v>2015</v>
       </c>
-      <c r="C46" s="4">
-        <v>98</v>
+      <c r="C46" s="20">
+        <v>45</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>267</v>
@@ -12177,8 +12216,8 @@
       <c r="B47" s="3">
         <v>2015</v>
       </c>
-      <c r="C47" s="4">
-        <v>99</v>
+      <c r="C47" s="20">
+        <v>46</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>273</v>
@@ -12219,8 +12258,8 @@
       <c r="B48" s="3">
         <v>2015</v>
       </c>
-      <c r="C48" s="4">
-        <v>100</v>
+      <c r="C48" s="20">
+        <v>47</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>279</v>
@@ -12261,8 +12300,8 @@
       <c r="B49" s="3">
         <v>2015</v>
       </c>
-      <c r="C49" s="4">
-        <v>104</v>
+      <c r="C49" s="20">
+        <v>48</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>285</v>
@@ -12303,8 +12342,8 @@
       <c r="B50" s="3">
         <v>2015</v>
       </c>
-      <c r="C50" s="4">
-        <v>1</v>
+      <c r="C50" s="20">
+        <v>49</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>292</v>
@@ -12345,8 +12384,8 @@
       <c r="B51" s="3">
         <v>2015</v>
       </c>
-      <c r="C51" s="4">
-        <v>2</v>
+      <c r="C51" s="20">
+        <v>50</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>298</v>
@@ -12387,8 +12426,8 @@
       <c r="B52" s="3">
         <v>2015</v>
       </c>
-      <c r="C52" s="4">
-        <v>3</v>
+      <c r="C52" s="19">
+        <v>51</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>304</v>
@@ -12429,8 +12468,8 @@
       <c r="B53" s="3">
         <v>2015</v>
       </c>
-      <c r="C53" s="4">
-        <v>4</v>
+      <c r="C53" s="20">
+        <v>52</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>310</v>
@@ -12471,8 +12510,8 @@
       <c r="B54" s="3">
         <v>2015</v>
       </c>
-      <c r="C54" s="4">
-        <v>5</v>
+      <c r="C54" s="20">
+        <v>53</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>316</v>
@@ -12513,8 +12552,8 @@
       <c r="B55" s="3">
         <v>2015</v>
       </c>
-      <c r="C55" s="4">
-        <v>13</v>
+      <c r="C55" s="20">
+        <v>54</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>322</v>
@@ -12555,8 +12594,8 @@
       <c r="B56" s="3">
         <v>2015</v>
       </c>
-      <c r="C56" s="4">
-        <v>96</v>
+      <c r="C56" s="20">
+        <v>55</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>328</v>
@@ -12597,8 +12636,8 @@
       <c r="B57" s="3">
         <v>2015</v>
       </c>
-      <c r="C57" s="4">
-        <v>97</v>
+      <c r="C57" s="20">
+        <v>56</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>334</v>
@@ -12639,8 +12678,8 @@
       <c r="B58" s="3">
         <v>2015</v>
       </c>
-      <c r="C58" s="4">
-        <v>98</v>
+      <c r="C58" s="20">
+        <v>57</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>340</v>
@@ -12681,8 +12720,8 @@
       <c r="B59" s="3">
         <v>2015</v>
       </c>
-      <c r="C59" s="4">
-        <v>99</v>
+      <c r="C59" s="20">
+        <v>58</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>346</v>
@@ -12723,8 +12762,8 @@
       <c r="B60" s="3">
         <v>2015</v>
       </c>
-      <c r="C60" s="4">
-        <v>100</v>
+      <c r="C60" s="20">
+        <v>59</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>352</v>
@@ -12765,8 +12804,8 @@
       <c r="B61" s="3">
         <v>2015</v>
       </c>
-      <c r="C61" s="4">
-        <v>102</v>
+      <c r="C61" s="20">
+        <v>60</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>358</v>
@@ -12807,8 +12846,8 @@
       <c r="B62" s="3">
         <v>2015</v>
       </c>
-      <c r="C62" s="4">
-        <v>103</v>
+      <c r="C62" s="20">
+        <v>61</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>364</v>
@@ -12849,8 +12888,8 @@
       <c r="B63" s="3">
         <v>2015</v>
       </c>
-      <c r="C63" s="4">
-        <v>104</v>
+      <c r="C63" s="20">
+        <v>62</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>370</v>
@@ -12891,8 +12930,8 @@
       <c r="B64" s="3">
         <v>2015</v>
       </c>
-      <c r="C64" s="4">
-        <v>105</v>
+      <c r="C64" s="20">
+        <v>63</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>376</v>
@@ -12933,8 +12972,8 @@
       <c r="B65" s="3">
         <v>2015</v>
       </c>
-      <c r="C65" s="4">
-        <v>106</v>
+      <c r="C65" s="20">
+        <v>64</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>376</v>
@@ -12975,8 +13014,8 @@
       <c r="B66" s="3">
         <v>2015</v>
       </c>
-      <c r="C66" s="4">
-        <v>109</v>
+      <c r="C66" s="20">
+        <v>65</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>387</v>
@@ -13017,8 +13056,8 @@
       <c r="B67" s="3">
         <v>2015</v>
       </c>
-      <c r="C67" s="4">
-        <v>110</v>
+      <c r="C67" s="20">
+        <v>66</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>393</v>
@@ -13059,8 +13098,8 @@
       <c r="B68" s="3">
         <v>2015</v>
       </c>
-      <c r="C68" s="4">
-        <v>111</v>
+      <c r="C68" s="20">
+        <v>67</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>399</v>
@@ -13101,8 +13140,8 @@
       <c r="B69" s="3">
         <v>2015</v>
       </c>
-      <c r="C69" s="4">
-        <v>112</v>
+      <c r="C69" s="20">
+        <v>68</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>376</v>
@@ -13143,8 +13182,8 @@
       <c r="B70" s="3">
         <v>2015</v>
       </c>
-      <c r="C70" s="4">
-        <v>113</v>
+      <c r="C70" s="20">
+        <v>69</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>410</v>
@@ -13185,8 +13224,8 @@
       <c r="B71" s="3">
         <v>2015</v>
       </c>
-      <c r="C71" s="4">
-        <v>115</v>
+      <c r="C71" s="20">
+        <v>70</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>416</v>
@@ -13227,8 +13266,8 @@
       <c r="B72" s="3">
         <v>2015</v>
       </c>
-      <c r="C72" s="4">
-        <v>116</v>
+      <c r="C72" s="20">
+        <v>71</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>376</v>
@@ -13269,8 +13308,8 @@
       <c r="B73" s="3">
         <v>2015</v>
       </c>
-      <c r="C73" s="4">
-        <v>117</v>
+      <c r="C73" s="20">
+        <v>72</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>376</v>
@@ -13311,8 +13350,8 @@
       <c r="B74" s="3">
         <v>2015</v>
       </c>
-      <c r="C74" s="4">
-        <v>119</v>
+      <c r="C74" s="20">
+        <v>73</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>432</v>
@@ -13353,8 +13392,8 @@
       <c r="B75" s="3">
         <v>2015</v>
       </c>
-      <c r="C75" s="4">
-        <v>8</v>
+      <c r="C75" s="20">
+        <v>74</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>439</v>
@@ -13395,8 +13434,8 @@
       <c r="B76" s="3">
         <v>2015</v>
       </c>
-      <c r="C76" s="4">
-        <v>13</v>
+      <c r="C76" s="20">
+        <v>75</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>445</v>
@@ -13437,8 +13476,8 @@
       <c r="B77" s="3">
         <v>2015</v>
       </c>
-      <c r="C77" s="4">
-        <v>17</v>
+      <c r="C77" s="19">
+        <v>76</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>451</v>
@@ -13479,8 +13518,8 @@
       <c r="B78" s="3">
         <v>2015</v>
       </c>
-      <c r="C78" s="4">
-        <v>19</v>
+      <c r="C78" s="20">
+        <v>77</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>457</v>
@@ -13521,8 +13560,8 @@
       <c r="B79" s="3">
         <v>2015</v>
       </c>
-      <c r="C79" s="4">
-        <v>24</v>
+      <c r="C79" s="20">
+        <v>78</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>463</v>
@@ -13563,8 +13602,8 @@
       <c r="B80" s="3">
         <v>2015</v>
       </c>
-      <c r="C80" s="4">
-        <v>37</v>
+      <c r="C80" s="20">
+        <v>79</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>465</v>
@@ -13605,8 +13644,8 @@
       <c r="B81" s="3">
         <v>2015</v>
       </c>
-      <c r="C81" s="4">
-        <v>39</v>
+      <c r="C81" s="20">
+        <v>80</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>471</v>
@@ -13647,8 +13686,8 @@
       <c r="B82" s="3">
         <v>2015</v>
       </c>
-      <c r="C82" s="4">
-        <v>41</v>
+      <c r="C82" s="20">
+        <v>81</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>477</v>
@@ -13689,8 +13728,8 @@
       <c r="B83" s="3">
         <v>2015</v>
       </c>
-      <c r="C83" s="4">
-        <v>42</v>
+      <c r="C83" s="20">
+        <v>82</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>483</v>
@@ -13731,8 +13770,8 @@
       <c r="B84" s="3">
         <v>2015</v>
       </c>
-      <c r="C84" s="4">
-        <v>43</v>
+      <c r="C84" s="20">
+        <v>83</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>485</v>
@@ -13773,8 +13812,8 @@
       <c r="B85" s="3">
         <v>2015</v>
       </c>
-      <c r="C85" s="4">
-        <v>52</v>
+      <c r="C85" s="20">
+        <v>84</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>491</v>
@@ -13815,8 +13854,8 @@
       <c r="B86" s="3">
         <v>2015</v>
       </c>
-      <c r="C86" s="4">
-        <v>53</v>
+      <c r="C86" s="20">
+        <v>85</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>497</v>
@@ -13857,8 +13896,8 @@
       <c r="B87" s="3">
         <v>2015</v>
       </c>
-      <c r="C87" s="4">
-        <v>63</v>
+      <c r="C87" s="20">
+        <v>86</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>502</v>
@@ -13899,8 +13938,8 @@
       <c r="B88" s="3">
         <v>2015</v>
       </c>
-      <c r="C88" s="4">
-        <v>65</v>
+      <c r="C88" s="20">
+        <v>87</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>508</v>
@@ -13941,8 +13980,8 @@
       <c r="B89" s="3">
         <v>2015</v>
       </c>
-      <c r="C89" s="4">
-        <v>7</v>
+      <c r="C89" s="20">
+        <v>88</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>514</v>
@@ -13983,8 +14022,8 @@
       <c r="B90" s="3">
         <v>2015</v>
       </c>
-      <c r="C90" s="4">
-        <v>69</v>
+      <c r="C90" s="20">
+        <v>89</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>520</v>
@@ -14025,8 +14064,8 @@
       <c r="B91" s="3">
         <v>2015</v>
       </c>
-      <c r="C91" s="4">
-        <v>91</v>
+      <c r="C91" s="20">
+        <v>90</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>526</v>
@@ -14067,8 +14106,8 @@
       <c r="B92" s="3">
         <v>2015</v>
       </c>
-      <c r="C92" s="4">
-        <v>92</v>
+      <c r="C92" s="20">
+        <v>91</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>532</v>
@@ -14109,8 +14148,8 @@
       <c r="B93" s="3">
         <v>2015</v>
       </c>
-      <c r="C93" s="4">
-        <v>93</v>
+      <c r="C93" s="20">
+        <v>92</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>538</v>
@@ -14151,8 +14190,8 @@
       <c r="B94" s="3">
         <v>2015</v>
       </c>
-      <c r="C94" s="4">
-        <v>96</v>
+      <c r="C94" s="20">
+        <v>93</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>544</v>
@@ -14193,8 +14232,8 @@
       <c r="B95" s="3">
         <v>2015</v>
       </c>
-      <c r="C95" s="4">
-        <v>99</v>
+      <c r="C95" s="20">
+        <v>94</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>550</v>
@@ -14235,8 +14274,8 @@
       <c r="B96" s="3">
         <v>2015</v>
       </c>
-      <c r="C96" s="4">
-        <v>113</v>
+      <c r="C96" s="20">
+        <v>95</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>556</v>
@@ -14277,8 +14316,8 @@
       <c r="B97" s="3">
         <v>2015</v>
       </c>
-      <c r="C97" s="4">
-        <v>1</v>
+      <c r="C97" s="20">
+        <v>96</v>
       </c>
       <c r="D97" s="7" t="s">
         <v>563</v>
@@ -14319,8 +14358,8 @@
       <c r="B98" s="3">
         <v>2015</v>
       </c>
-      <c r="C98" s="4">
-        <v>2</v>
+      <c r="C98" s="20">
+        <v>97</v>
       </c>
       <c r="D98" s="7" t="s">
         <v>569</v>
@@ -14361,8 +14400,8 @@
       <c r="B99" s="3">
         <v>2015</v>
       </c>
-      <c r="C99" s="4">
-        <v>3</v>
+      <c r="C99" s="20">
+        <v>98</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>575</v>
@@ -14403,8 +14442,8 @@
       <c r="B100" s="3">
         <v>2015</v>
       </c>
-      <c r="C100" s="4">
-        <v>4</v>
+      <c r="C100" s="20">
+        <v>99</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>581</v>
@@ -14445,8 +14484,8 @@
       <c r="B101" s="3">
         <v>2015</v>
       </c>
-      <c r="C101" s="4">
-        <v>5</v>
+      <c r="C101" s="20">
+        <v>100</v>
       </c>
       <c r="D101" s="7" t="s">
         <v>587</v>
@@ -14487,8 +14526,8 @@
       <c r="B102" s="3">
         <v>2015</v>
       </c>
-      <c r="C102" s="4">
-        <v>6</v>
+      <c r="C102" s="19">
+        <v>101</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>593</v>
@@ -14529,8 +14568,8 @@
       <c r="B103" s="3">
         <v>2015</v>
       </c>
-      <c r="C103" s="4">
-        <v>7</v>
+      <c r="C103" s="20">
+        <v>102</v>
       </c>
       <c r="D103" s="7" t="s">
         <v>599</v>
@@ -14571,8 +14610,8 @@
       <c r="B104" s="3">
         <v>2015</v>
       </c>
-      <c r="C104" s="4">
-        <v>8</v>
+      <c r="C104" s="20">
+        <v>103</v>
       </c>
       <c r="D104" s="7" t="s">
         <v>605</v>
@@ -14613,8 +14652,8 @@
       <c r="B105" s="3">
         <v>2015</v>
       </c>
-      <c r="C105" s="4">
-        <v>9</v>
+      <c r="C105" s="20">
+        <v>104</v>
       </c>
       <c r="D105" s="7" t="s">
         <v>611</v>
@@ -14655,8 +14694,8 @@
       <c r="B106" s="3">
         <v>2015</v>
       </c>
-      <c r="C106" s="4">
-        <v>10</v>
+      <c r="C106" s="20">
+        <v>105</v>
       </c>
       <c r="D106" s="7" t="s">
         <v>617</v>
@@ -14697,8 +14736,8 @@
       <c r="B107" s="3">
         <v>2015</v>
       </c>
-      <c r="C107" s="4">
-        <v>11</v>
+      <c r="C107" s="20">
+        <v>106</v>
       </c>
       <c r="D107" s="7" t="s">
         <v>623</v>
@@ -14739,8 +14778,8 @@
       <c r="B108" s="3">
         <v>2015</v>
       </c>
-      <c r="C108" s="4">
-        <v>12</v>
+      <c r="C108" s="20">
+        <v>107</v>
       </c>
       <c r="D108" s="7" t="s">
         <v>629</v>
@@ -14781,8 +14820,8 @@
       <c r="B109" s="3">
         <v>2015</v>
       </c>
-      <c r="C109" s="4">
-        <v>112</v>
+      <c r="C109" s="20">
+        <v>108</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>636</v>
@@ -14823,8 +14862,8 @@
       <c r="B110" s="3">
         <v>2015</v>
       </c>
-      <c r="C110" s="4">
-        <v>54</v>
+      <c r="C110" s="20">
+        <v>109</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>643</v>
@@ -14865,8 +14904,8 @@
       <c r="B111" s="3">
         <v>2015</v>
       </c>
-      <c r="C111" s="4">
-        <v>55</v>
+      <c r="C111" s="20">
+        <v>110</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>649</v>
@@ -14907,8 +14946,8 @@
       <c r="B112" s="3">
         <v>2015</v>
       </c>
-      <c r="C112" s="4">
-        <v>56</v>
+      <c r="C112" s="20">
+        <v>111</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>655</v>
@@ -14949,8 +14988,8 @@
       <c r="B113" s="3">
         <v>2015</v>
       </c>
-      <c r="C113" s="4">
-        <v>57</v>
+      <c r="C113" s="20">
+        <v>112</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>661</v>
@@ -14991,8 +15030,8 @@
       <c r="B114" s="3">
         <v>2015</v>
       </c>
-      <c r="C114" s="4">
-        <v>58</v>
+      <c r="C114" s="20">
+        <v>113</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>667</v>
@@ -15033,8 +15072,8 @@
       <c r="B115" s="3">
         <v>2015</v>
       </c>
-      <c r="C115" s="4">
-        <v>59</v>
+      <c r="C115" s="20">
+        <v>114</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>673</v>
@@ -15075,8 +15114,8 @@
       <c r="B116" s="3">
         <v>2015</v>
       </c>
-      <c r="C116" s="4">
-        <v>60</v>
+      <c r="C116" s="20">
+        <v>115</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>679</v>
@@ -15117,8 +15156,8 @@
       <c r="B117" s="3">
         <v>2015</v>
       </c>
-      <c r="C117" s="4">
-        <v>61</v>
+      <c r="C117" s="20">
+        <v>116</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>685</v>
@@ -15159,8 +15198,8 @@
       <c r="B118" s="3">
         <v>2015</v>
       </c>
-      <c r="C118" s="4">
-        <v>62</v>
+      <c r="C118" s="20">
+        <v>117</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>691</v>
@@ -15201,8 +15240,8 @@
       <c r="B119" s="3">
         <v>2015</v>
       </c>
-      <c r="C119" s="4">
-        <v>63</v>
+      <c r="C119" s="20">
+        <v>118</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>697</v>
@@ -15243,8 +15282,8 @@
       <c r="B120" s="3">
         <v>2015</v>
       </c>
-      <c r="C120" s="4">
-        <v>64</v>
+      <c r="C120" s="20">
+        <v>119</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>703</v>
@@ -15285,8 +15324,8 @@
       <c r="B121" s="3">
         <v>2015</v>
       </c>
-      <c r="C121" s="4">
-        <v>65</v>
+      <c r="C121" s="20">
+        <v>120</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>709</v>
@@ -15327,8 +15366,8 @@
       <c r="B122" s="3">
         <v>2015</v>
       </c>
-      <c r="C122" s="4">
-        <v>81</v>
+      <c r="C122" s="20">
+        <v>121</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>715</v>
@@ -15369,8 +15408,8 @@
       <c r="B123" s="3">
         <v>2015</v>
       </c>
-      <c r="C123" s="4">
-        <v>82</v>
+      <c r="C123" s="20">
+        <v>122</v>
       </c>
       <c r="D123" s="5" t="s">
         <v>376</v>
@@ -15411,8 +15450,8 @@
       <c r="B124" s="3">
         <v>2015</v>
       </c>
-      <c r="C124" s="4">
-        <v>83</v>
+      <c r="C124" s="20">
+        <v>123</v>
       </c>
       <c r="D124" s="5" t="s">
         <v>726</v>
@@ -15453,8 +15492,8 @@
       <c r="B125" s="3">
         <v>2015</v>
       </c>
-      <c r="C125" s="4">
-        <v>84</v>
+      <c r="C125" s="20">
+        <v>124</v>
       </c>
       <c r="D125" s="5" t="s">
         <v>358</v>
@@ -15495,8 +15534,8 @@
       <c r="B126" s="3">
         <v>2015</v>
       </c>
-      <c r="C126" s="4">
-        <v>85</v>
+      <c r="C126" s="20">
+        <v>125</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>737</v>
@@ -15537,8 +15576,8 @@
       <c r="B127" s="3">
         <v>2015</v>
       </c>
-      <c r="C127" s="4">
-        <v>86</v>
+      <c r="C127" s="19">
+        <v>126</v>
       </c>
       <c r="D127" s="5" t="s">
         <v>743</v>
@@ -15579,8 +15618,8 @@
       <c r="B128" s="3">
         <v>2015</v>
       </c>
-      <c r="C128" s="4">
-        <v>87</v>
+      <c r="C128" s="20">
+        <v>127</v>
       </c>
       <c r="D128" s="5" t="s">
         <v>748</v>
@@ -15621,8 +15660,8 @@
       <c r="B129" s="3">
         <v>2015</v>
       </c>
-      <c r="C129" s="4">
-        <v>88</v>
+      <c r="C129" s="20">
+        <v>128</v>
       </c>
       <c r="D129" s="5" t="s">
         <v>754</v>
@@ -15663,8 +15702,8 @@
       <c r="B130" s="3">
         <v>2015</v>
       </c>
-      <c r="C130" s="4">
-        <v>89</v>
+      <c r="C130" s="20">
+        <v>129</v>
       </c>
       <c r="D130" s="5" t="s">
         <v>760</v>
@@ -15705,8 +15744,8 @@
       <c r="B131" s="3">
         <v>2015</v>
       </c>
-      <c r="C131" s="4">
-        <v>90</v>
+      <c r="C131" s="20">
+        <v>130</v>
       </c>
       <c r="D131" s="5" t="s">
         <v>766</v>
@@ -15747,8 +15786,8 @@
       <c r="B132" s="3">
         <v>2015</v>
       </c>
-      <c r="C132" s="4">
-        <v>91</v>
+      <c r="C132" s="20">
+        <v>131</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>772</v>
@@ -15789,8 +15828,8 @@
       <c r="B133" s="3">
         <v>2015</v>
       </c>
-      <c r="C133" s="4">
-        <v>92</v>
+      <c r="C133" s="20">
+        <v>132</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>778</v>
@@ -15831,8 +15870,8 @@
       <c r="B134" s="3">
         <v>2015</v>
       </c>
-      <c r="C134" s="4">
-        <v>93</v>
+      <c r="C134" s="20">
+        <v>133</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>784</v>
@@ -15873,8 +15912,8 @@
       <c r="B135" s="3">
         <v>2015</v>
       </c>
-      <c r="C135" s="4">
-        <v>94</v>
+      <c r="C135" s="20">
+        <v>134</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>790</v>
@@ -15915,8 +15954,8 @@
       <c r="B136" s="3">
         <v>2015</v>
       </c>
-      <c r="C136" s="4">
-        <v>95</v>
+      <c r="C136" s="20">
+        <v>135</v>
       </c>
       <c r="D136" s="5" t="s">
         <v>796</v>
@@ -15957,8 +15996,8 @@
       <c r="B137" s="3">
         <v>2015</v>
       </c>
-      <c r="C137" s="4">
-        <v>96</v>
+      <c r="C137" s="20">
+        <v>136</v>
       </c>
       <c r="D137" s="5" t="s">
         <v>801</v>
@@ -15999,8 +16038,8 @@
       <c r="B138" s="3">
         <v>2015</v>
       </c>
-      <c r="C138" s="4">
-        <v>97</v>
+      <c r="C138" s="20">
+        <v>137</v>
       </c>
       <c r="D138" s="5" t="s">
         <v>807</v>
@@ -16041,8 +16080,8 @@
       <c r="B139" s="3">
         <v>2015</v>
       </c>
-      <c r="C139" s="4">
-        <v>98</v>
+      <c r="C139" s="20">
+        <v>138</v>
       </c>
       <c r="D139" s="5" t="s">
         <v>813</v>
@@ -16083,8 +16122,8 @@
       <c r="B140" s="3">
         <v>2015</v>
       </c>
-      <c r="C140" s="4">
-        <v>99</v>
+      <c r="C140" s="20">
+        <v>139</v>
       </c>
       <c r="D140" s="5" t="s">
         <v>819</v>
@@ -16125,8 +16164,8 @@
       <c r="B141" s="3">
         <v>2015</v>
       </c>
-      <c r="C141" s="4">
-        <v>100</v>
+      <c r="C141" s="20">
+        <v>140</v>
       </c>
       <c r="D141" s="5" t="s">
         <v>825</v>
@@ -16167,8 +16206,8 @@
       <c r="B142" s="3">
         <v>2015</v>
       </c>
-      <c r="C142" s="4">
-        <v>101</v>
+      <c r="C142" s="20">
+        <v>141</v>
       </c>
       <c r="D142" s="5" t="s">
         <v>831</v>
@@ -16209,8 +16248,8 @@
       <c r="B143" s="3">
         <v>2015</v>
       </c>
-      <c r="C143" s="4">
-        <v>102</v>
+      <c r="C143" s="20">
+        <v>142</v>
       </c>
       <c r="D143" s="5" t="s">
         <v>834</v>
@@ -16251,8 +16290,8 @@
       <c r="B144" s="3">
         <v>2015</v>
       </c>
-      <c r="C144" s="4">
-        <v>103</v>
+      <c r="C144" s="20">
+        <v>143</v>
       </c>
       <c r="D144" s="5" t="s">
         <v>840</v>
@@ -16293,8 +16332,8 @@
       <c r="B145" s="3">
         <v>2015</v>
       </c>
-      <c r="C145" s="4">
-        <v>104</v>
+      <c r="C145" s="20">
+        <v>144</v>
       </c>
       <c r="D145" s="5" t="s">
         <v>845</v>
@@ -16335,8 +16374,8 @@
       <c r="B146" s="3">
         <v>2015</v>
       </c>
-      <c r="C146" s="4">
-        <v>105</v>
+      <c r="C146" s="20">
+        <v>145</v>
       </c>
       <c r="D146" s="5" t="s">
         <v>851</v>
@@ -16377,8 +16416,8 @@
       <c r="B147" s="3">
         <v>2015</v>
       </c>
-      <c r="C147" s="4">
-        <v>106</v>
+      <c r="C147" s="20">
+        <v>146</v>
       </c>
       <c r="D147" s="5" t="s">
         <v>857</v>
@@ -16419,8 +16458,8 @@
       <c r="B148" s="3">
         <v>2015</v>
       </c>
-      <c r="C148" s="4">
-        <v>107</v>
+      <c r="C148" s="20">
+        <v>147</v>
       </c>
       <c r="D148" s="5" t="s">
         <v>863</v>
@@ -16461,8 +16500,8 @@
       <c r="B149" s="3">
         <v>2015</v>
       </c>
-      <c r="C149" s="4">
-        <v>108</v>
+      <c r="C149" s="20">
+        <v>148</v>
       </c>
       <c r="D149" s="5" t="s">
         <v>869</v>
@@ -16503,8 +16542,8 @@
       <c r="B150" s="3">
         <v>2015</v>
       </c>
-      <c r="C150" s="4">
-        <v>109</v>
+      <c r="C150" s="20">
+        <v>149</v>
       </c>
       <c r="D150" s="5" t="s">
         <v>874</v>
@@ -16545,8 +16584,8 @@
       <c r="B151" s="3">
         <v>2015</v>
       </c>
-      <c r="C151" s="4">
-        <v>110</v>
+      <c r="C151" s="20">
+        <v>150</v>
       </c>
       <c r="D151" s="5" t="s">
         <v>880</v>

</xml_diff>